<commit_message>
Projection info is added
Calculate the generated shapefile file space coordinate information supplement.
</commit_message>
<xml_diff>
--- a/assets/test/TaiHang/result/indices.xlsx
+++ b/assets/test/TaiHang/result/indices.xlsx
@@ -91,7 +91,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="11.7109375" customWidth="true"/>
     <col min="6" max="6" width="11.7109375" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
@@ -141,10 +141,10 @@
         <v>2.1095154285430908</v>
       </c>
       <c r="G2" s="0">
-        <v>0.29551884531974792</v>
+        <v>2.955188512802124</v>
       </c>
       <c r="H2" s="0">
-        <v>1.8333333730697632</v>
+        <v>2.1666667461395264</v>
       </c>
     </row>
     <row r="3">
@@ -167,10 +167,10 @@
         <v>0.94329321384429932</v>
       </c>
       <c r="G3" s="0">
-        <v>0.35307338833808899</v>
+        <v>3.530733585357666</v>
       </c>
       <c r="H3" s="0">
-        <v>2.1666667461395264</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>